<commit_message>
adding max flight time making code more generic
</commit_message>
<xml_diff>
--- a/input2.xlsx
+++ b/input2.xlsx
@@ -7,15 +7,16 @@
     <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
   </bookViews>
   <sheets>
-    <sheet name="targets" sheetId="1" r:id="rId1"/>
-    <sheet name="agent2sensors" sheetId="2" r:id="rId2"/>
+    <sheet name="agent2sensors" sheetId="3" r:id="rId1"/>
+    <sheet name="targets" sheetId="1" r:id="rId2"/>
+    <sheet name="agent2sensorsOld" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>sensor</t>
   </si>
@@ -385,10 +386,182 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="A2:E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -908,12 +1081,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>